<commit_message>
add category and tags
</commit_message>
<xml_diff>
--- a/uploads/template_mapel.xlsx
+++ b/uploads/template_mapel.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS-A407M\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="30" windowWidth="22995" windowHeight="10050"/>
   </bookViews>
@@ -21,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Nama Mata Pelajaran</t>
   </si>
@@ -29,28 +24,22 @@
     <t>Kode Mata Pelajaran</t>
   </si>
   <si>
-    <t>bahasa indonesia</t>
-  </si>
-  <si>
-    <t>matematika</t>
-  </si>
-  <si>
-    <t>pancasila</t>
-  </si>
-  <si>
     <t>bahasa inggris</t>
   </si>
   <si>
-    <t>bin</t>
-  </si>
-  <si>
-    <t>mtk</t>
-  </si>
-  <si>
-    <t>ppkn</t>
-  </si>
-  <si>
     <t>big</t>
+  </si>
+  <si>
+    <t>pendidikan kewarganegaraan</t>
+  </si>
+  <si>
+    <t>pkn</t>
+  </si>
+  <si>
+    <t>pendidikan agama islam</t>
+  </si>
+  <si>
+    <t>pai</t>
   </si>
 </sst>
 </file>
@@ -98,9 +87,6 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -148,7 +134,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -183,7 +169,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -392,10 +378,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -413,31 +399,23 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix bug add edit view post
</commit_message>
<xml_diff>
--- a/uploads/template_mapel.xlsx
+++ b/uploads/template_mapel.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
   <si>
     <t>Nama Mata Pelajaran</t>
   </si>
@@ -29,28 +29,67 @@
     <t>Kode Mata Pelajaran</t>
   </si>
   <si>
-    <t>bahasa indonesia</t>
-  </si>
-  <si>
-    <t>matematika</t>
-  </si>
-  <si>
-    <t>pancasila</t>
-  </si>
-  <si>
-    <t>bahasa inggris</t>
-  </si>
-  <si>
-    <t>bin</t>
-  </si>
-  <si>
-    <t>mtk</t>
-  </si>
-  <si>
-    <t>ppkn</t>
-  </si>
-  <si>
-    <t>big</t>
+    <t>PPKN</t>
+  </si>
+  <si>
+    <t>Bahasa Indonesia</t>
+  </si>
+  <si>
+    <t>Matematika</t>
+  </si>
+  <si>
+    <t>IPA</t>
+  </si>
+  <si>
+    <t>IPS</t>
+  </si>
+  <si>
+    <t>Bahasa Inggris</t>
+  </si>
+  <si>
+    <t>Seni Budaya</t>
+  </si>
+  <si>
+    <t>Penjas Orkes</t>
+  </si>
+  <si>
+    <t>Prakarya</t>
+  </si>
+  <si>
+    <t>Bahasa Jawa (muatan lokal)</t>
+  </si>
+  <si>
+    <t>Pengembangan Diri(BK)</t>
+  </si>
+  <si>
+    <t>Pend. Agama &amp; Budi Pekerti</t>
+  </si>
+  <si>
+    <t>PA</t>
+  </si>
+  <si>
+    <t>BIN</t>
+  </si>
+  <si>
+    <t>MTK</t>
+  </si>
+  <si>
+    <t>BIG</t>
+  </si>
+  <si>
+    <t>SB</t>
+  </si>
+  <si>
+    <t>OR</t>
+  </si>
+  <si>
+    <t>PK</t>
+  </si>
+  <si>
+    <t>BJ</t>
+  </si>
+  <si>
+    <t>BK</t>
   </si>
 </sst>
 </file>
@@ -392,10 +431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -410,38 +449,103 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="70" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>